<commit_message>
material model calculations for brick
</commit_message>
<xml_diff>
--- a/Measurements/cube_data_finalProject.xlsx
+++ b/Measurements/cube_data_finalProject.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="13395" windowHeight="5700"/>
+    <workbookView xWindow="-1770" yWindow="-180" windowWidth="13395" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +16,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Initial weight (kg)</t>
   </si>
   <si>
     <t>Initial Displace (inches)</t>
+  </si>
+  <si>
+    <t>1.5x1.5</t>
+  </si>
+  <si>
+    <t>0.036/0.785</t>
+  </si>
+  <si>
+    <t>0.061/0.785</t>
+  </si>
+  <si>
+    <t>0.067/0.785</t>
+  </si>
+  <si>
+    <t>0.09/0.785</t>
+  </si>
+  <si>
+    <t>0.099/0.785</t>
+  </si>
+  <si>
+    <t>0.133/0.785</t>
+  </si>
+  <si>
+    <t>0.183/0.785</t>
+  </si>
+  <si>
+    <t>0.328/2.25</t>
+  </si>
+  <si>
+    <t>0.72/2.25</t>
+  </si>
+  <si>
+    <t>0.969/2.25</t>
+  </si>
+  <si>
+    <t>1.24/2.25</t>
+  </si>
+  <si>
+    <t>1.78/2.25</t>
+  </si>
+  <si>
+    <t>3.15/2.25</t>
+  </si>
+  <si>
+    <t>5.27/2.25</t>
+  </si>
+  <si>
+    <t>Stiffness = 12.046 Newton/inches^2 = 18671.3 pascals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lambda = 1.077 × 104 Pa
+</t>
+  </si>
+  <si>
+    <t>mu = 7181 Pa</t>
   </si>
 </sst>
 </file>
@@ -57,9 +112,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -72,6 +130,200 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$20:$D$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.5859999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.7706999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5349999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11465</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.126115</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16942699999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23312099999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$20:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.14577799999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43066700000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.55111100000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.79111100000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.342222</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="81143296"/>
+        <c:axId val="81141760"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="81143296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81141760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="81141760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81143296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>338137</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -361,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,13 +729,144 @@
         <v>5.27</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>0.78500000000000003</v>
       </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>4.5859999999999998E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.14577799999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>7.7706999999999998E-2</v>
+      </c>
+      <c r="E21">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>8.5349999999999995E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.43066700000000002</v>
+      </c>
+      <c r="I22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>0.11465</v>
+      </c>
+      <c r="E23">
+        <v>0.55111100000000002</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>0.126115</v>
+      </c>
+      <c r="E24">
+        <v>0.79111100000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>0.16942699999999999</v>
+      </c>
+      <c r="E25">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>0.23312099999999999</v>
+      </c>
+      <c r="E26">
+        <v>2.342222</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
finished recreating cube experiment
</commit_message>
<xml_diff>
--- a/Measurements/cube_data_finalProject.xlsx
+++ b/Measurements/cube_data_finalProject.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Initial weight (kg)</t>
   </si>
@@ -24,9 +24,6 @@
     <t>Initial Displace (inches)</t>
   </si>
   <si>
-    <t>1.5x1.5</t>
-  </si>
-  <si>
     <t>0.036/0.785</t>
   </si>
   <si>
@@ -48,35 +45,71 @@
     <t>0.183/0.785</t>
   </si>
   <si>
-    <t>0.328/2.25</t>
-  </si>
-  <si>
-    <t>0.72/2.25</t>
-  </si>
-  <si>
-    <t>0.969/2.25</t>
-  </si>
-  <si>
-    <t>1.24/2.25</t>
-  </si>
-  <si>
-    <t>1.78/2.25</t>
-  </si>
-  <si>
-    <t>3.15/2.25</t>
-  </si>
-  <si>
-    <t>5.27/2.25</t>
-  </si>
-  <si>
-    <t>Stiffness = 12.046 Newton/inches^2 = 18671.3 pascals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lambda = 1.077 × 104 Pa
+    <t>0.328/2.25*9.8</t>
+  </si>
+  <si>
+    <t>0.72/2.25*9.8</t>
+  </si>
+  <si>
+    <t>0.969/2.25*9.8</t>
+  </si>
+  <si>
+    <t>1.24/2.25*9.8</t>
+  </si>
+  <si>
+    <t>1.78/2.25*9.8</t>
+  </si>
+  <si>
+    <t>3.15/2.25*9.8</t>
+  </si>
+  <si>
+    <t>5.27/2.25*9.8</t>
+  </si>
+  <si>
+    <t>Stiffness = 12.046 Newton/inches^2 = 182979 pascals</t>
+  </si>
+  <si>
+    <t>mu = 7.038*10^4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lambda = 1.056 10^5 Pa
 </t>
   </si>
   <si>
-    <t>mu = 7181 Pa</t>
+    <t>init 123</t>
+  </si>
+  <si>
+    <t>fin 123</t>
+  </si>
+  <si>
+    <t>delta m</t>
+  </si>
+  <si>
+    <t>delta inches</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>force kg</t>
+  </si>
+  <si>
+    <t>0.785 inches = 0.019939 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5inch square = 0.0381 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">init </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fin </t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>UNSTABLE!!</t>
   </si>
 </sst>
 </file>
@@ -112,11 +145,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -201,30 +237,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$20:$E$26</c:f>
+              <c:f>Sheet1!$F$20:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.14577799999999999</c:v>
+                  <c:v>1.4286243999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32</c:v>
+                  <c:v>3.1360000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.43066700000000002</c:v>
+                  <c:v>4.2205366000000009</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55111100000000002</c:v>
+                  <c:v>5.4008878000000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79111100000000001</c:v>
+                  <c:v>7.7528878000000008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4</c:v>
+                  <c:v>13.72</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.342222</c:v>
+                  <c:v>22.9537756</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -239,11 +275,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="81143296"/>
-        <c:axId val="81141760"/>
+        <c:axId val="52900608"/>
+        <c:axId val="52894720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81143296"/>
+        <c:axId val="52900608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -253,12 +289,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81141760"/>
+        <c:crossAx val="52894720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81141760"/>
+        <c:axId val="52894720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -269,7 +305,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81143296"/>
+        <c:crossAx val="52900608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -295,20 +331,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>338137</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -616,7 +652,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,64 +775,64 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.25">
@@ -806,6 +842,10 @@
       <c r="E20">
         <v>0.14577799999999999</v>
       </c>
+      <c r="F20">
+        <f xml:space="preserve"> 9.8 *E20:E26</f>
+        <v>1.4286243999999999</v>
+      </c>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D21">
@@ -814,6 +854,10 @@
       <c r="E21">
         <v>0.32</v>
       </c>
+      <c r="F21">
+        <f t="shared" ref="F21:F26" si="0" xml:space="preserve"> 9.8 *E21:E27</f>
+        <v>3.1360000000000001</v>
+      </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D22">
@@ -822,8 +866,12 @@
       <c r="E22">
         <v>0.43066700000000002</v>
       </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>4.2205366000000009</v>
+      </c>
       <c r="I22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="4:10" ht="60" x14ac:dyDescent="0.25">
@@ -833,11 +881,15 @@
       <c r="E23">
         <v>0.55111100000000002</v>
       </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>5.4008878000000005</v>
+      </c>
       <c r="I23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.25">
@@ -847,6 +899,10 @@
       <c r="E24">
         <v>0.79111100000000001</v>
       </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>7.7528878000000008</v>
+      </c>
     </row>
     <row r="25" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D25">
@@ -855,6 +911,10 @@
       <c r="E25">
         <v>1.4</v>
       </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>13.72</v>
+      </c>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D26">
@@ -862,6 +922,10 @@
       </c>
       <c r="E26">
         <v>2.342222</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>22.9537756</v>
       </c>
     </row>
   </sheetData>
@@ -872,13 +936,175 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>2.886E-2</v>
+      </c>
+      <c r="B1">
+        <v>2.6654000000000001E-2</v>
+      </c>
+      <c r="C1">
+        <v>2.2060000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.72</v>
+      </c>
+      <c r="B8">
+        <v>2.886E-2</v>
+      </c>
+      <c r="C8">
+        <v>2.6654000000000001E-2</v>
+      </c>
+      <c r="D8">
+        <v>2.2060000000000001E-3</v>
+      </c>
+      <c r="E8">
+        <v>8.6849999999999997E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.72</v>
+      </c>
+      <c r="B14">
+        <v>1.9938999999999998E-2</v>
+      </c>
+      <c r="C14">
+        <v>1.86669E-2</v>
+      </c>
+      <c r="D14">
+        <v>1.2719999999999999E-3</v>
+      </c>
+      <c r="E14">
+        <v>5.0083000000000003E-2</v>
+      </c>
+      <c r="G14">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>0.186803</v>
+      </c>
+      <c r="D15">
+        <v>1.2589999999999999E-3</v>
+      </c>
+      <c r="E15">
+        <v>4.9555000000000002E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1.2430000000000001</v>
+      </c>
+      <c r="B16">
+        <v>1.9938999999999998E-2</v>
+      </c>
+      <c r="C16">
+        <v>1.7906499999999999E-2</v>
+      </c>
+      <c r="D16">
+        <v>2.0330000000000001E-3</v>
+      </c>
+      <c r="E16">
+        <v>8.0019999999999994E-2</v>
+      </c>
+      <c r="G16">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1.78</v>
+      </c>
+      <c r="B17">
+        <v>1.9938999999999998E-2</v>
+      </c>
+      <c r="C17">
+        <v>1.72696E-2</v>
+      </c>
+      <c r="D17">
+        <v>2.6689999999999999E-3</v>
+      </c>
+      <c r="E17">
+        <v>0.10507900000000001</v>
+      </c>
+      <c r="G17">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3.15</v>
+      </c>
+      <c r="B18">
+        <v>1.9938999999999998E-2</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C18:F18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
finished final presentation slides
</commit_message>
<xml_diff>
--- a/Measurements/cube_data_finalProject.xlsx
+++ b/Measurements/cube_data_finalProject.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-1770" yWindow="-180" windowWidth="13395" windowHeight="5700"/>
+    <workbookView xWindow="-1770" yWindow="-180" windowWidth="13395" windowHeight="5700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,11 +275,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="52900608"/>
-        <c:axId val="52894720"/>
+        <c:axId val="123087104"/>
+        <c:axId val="123088896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52900608"/>
+        <c:axId val="123087104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -289,12 +289,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52894720"/>
+        <c:crossAx val="123088896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52894720"/>
+        <c:axId val="123088896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -305,7 +305,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52900608"/>
+        <c:crossAx val="123087104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -651,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,9 +936,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -1098,6 +1098,17 @@
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="B19">
+        <v>1.9938999999999998E-2</v>
+      </c>
+      <c r="G19">
+        <v>3.5999999999999997E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
one more data point for simulated cube experiment
</commit_message>
<xml_diff>
--- a/Measurements/cube_data_finalProject.xlsx
+++ b/Measurements/cube_data_finalProject.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-1770" yWindow="-180" windowWidth="13395" windowHeight="5700" activeTab="1"/>
+    <workbookView xWindow="-1770" yWindow="-180" windowWidth="13395" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -651,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -938,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,6 +1105,15 @@
       </c>
       <c r="B19">
         <v>1.9938999999999998E-2</v>
+      </c>
+      <c r="C19">
+        <v>1.9339700000000001E-2</v>
+      </c>
+      <c r="D19">
+        <v>5.9299999999999999E-4</v>
+      </c>
+      <c r="E19">
+        <v>2.3599999999999999E-2</v>
       </c>
       <c r="G19">
         <v>3.5999999999999997E-2</v>
@@ -1123,7 +1132,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>